<commit_message>
updated naming conventions in code and Excel file as needed
</commit_message>
<xml_diff>
--- a/data/raw/Industries by Impact Groupings.xlsx
+++ b/data/raw/Industries by Impact Groupings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://castatelibrary.sharepoint.com/sites/CRB2-CRB-MEISTeaminc.Tom/Shared Documents/CRB - MEIS Team inc. Tom/2021_MEIS/Mastersheets_Code/County_Mastersheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumeet.bedi\Documents\R\MEIS\meis_post-implan_mastersheets\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{C55E37C9-637C-944F-91B6-ED30AA28FFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A64EEC0-E2E6-48E5-B988-FEC56460F601}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C124F858-AA04-4D37-924D-A773B33A3BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12630" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16170" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="561">
   <si>
     <t>Oilseed farming</t>
   </si>
@@ -1716,6 +1716,9 @@
   </si>
   <si>
     <t>rollup</t>
+  </si>
+  <si>
+    <t>Accommodations</t>
   </si>
 </sst>
 </file>
@@ -1786,9 +1789,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1826,9 +1829,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1861,26 +1864,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1913,26 +1899,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2108,9 +2077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C535"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B542" sqref="B542"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7703,7 +7670,7 @@
         <v>516</v>
       </c>
       <c r="C508" t="s">
-        <v>517</v>
+        <v>560</v>
       </c>
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.3">
@@ -7714,7 +7681,7 @@
         <v>518</v>
       </c>
       <c r="C509" t="s">
-        <v>517</v>
+        <v>560</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.3">
@@ -9050,33 +9017,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="5aff56ac-f36b-49b3-8eea-e42fc37821cb">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="5aff56ac-f36b-49b3-8eea-e42fc37821cb" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e750500f-42a5-4b8d-9659-3e1833e664de">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100553AAAAFA06B6240B39104FB8E692371" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="92b4d3d33e1da38c95fab6da0116754d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e750500f-42a5-4b8d-9659-3e1833e664de" xmlns:ns3="5aff56ac-f36b-49b3-8eea-e42fc37821cb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f9d203eae2c29521611641dfe4a7cbe" ns2:_="" ns3:_="">
     <xsd:import namespace="e750500f-42a5-4b8d-9659-3e1833e664de"/>
@@ -9287,26 +9227,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13B1C32A-08D2-42F8-8450-14056F69FD1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5aff56ac-f36b-49b3-8eea-e42fc37821cb"/>
-    <ds:schemaRef ds:uri="e750500f-42a5-4b8d-9659-3e1833e664de"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B52E5306-3843-4C4C-BC6D-7F433E9C13FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="5aff56ac-f36b-49b3-8eea-e42fc37821cb">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="5aff56ac-f36b-49b3-8eea-e42fc37821cb" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e750500f-42a5-4b8d-9659-3e1833e664de">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21010A01-BA21-4A7A-9622-AAF8D92F2CAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9323,4 +9271,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B52E5306-3843-4C4C-BC6D-7F433E9C13FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13B1C32A-08D2-42F8-8450-14056F69FD1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5aff56ac-f36b-49b3-8eea-e42fc37821cb"/>
+    <ds:schemaRef ds:uri="e750500f-42a5-4b8d-9659-3e1833e664de"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>